<commit_message>
Added Delete function in transactions.html
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="340" yWindow="2240" windowWidth="17820" windowHeight="11770" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Spent" sheetId="1" state="visible" r:id="rId1"/>
@@ -413,14 +413,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
+    <col width="21.08984375" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="12.08984375" bestFit="1" customWidth="1" min="3" max="3"/>
     <col width="13.453125" bestFit="1" customWidth="1" min="4" max="4"/>
     <col width="18.54296875" bestFit="1" customWidth="1" min="5" max="5"/>
@@ -548,37 +549,37 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>20241205163526997030</t>
+          <t>20241205165544011465</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2024-08-22</t>
+          <t>2018-09-24</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>73.95999999999999</v>
+        <v>23.25</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>RDS PETROZA</t>
+          <t>Berjaya Starbucks Coffee Company SDN BHD</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Others</t>
+          <t>Food</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>20241205165544011465</t>
+          <t>20241205195645148493</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2018-09-24</t>
+          <t>2024-12-04</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -586,7 +587,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Berjaya Starbucks Coffee Company SDN BHD</t>
+          <t>Berjaya Starbucks Coffee Company Sdn Bhd</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -598,20 +599,20 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>20241205173730853658</t>
+          <t>20241205200912328800</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2018-09-24</t>
+          <t>2024-12-01</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>3023.25</v>
+        <v>23.25</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Berjaya Starbucks Coffee Company Sdn Bhd</t>
+          <t>KFC</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -623,98 +624,23 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>20241205195645148493</t>
+          <t>20241205201244653339</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2024-12-04</t>
+          <t>2024-12-20</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>23.25</v>
+        <v>100</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Berjaya Starbucks Coffee Company Sdn Bhd</t>
+          <t>Mcd</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
-        <is>
-          <t>Food</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>20241205200912328800</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2024-12-01</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>23.25</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>KFC</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Food</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>20241205201244653339</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>2024-12-20</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>100</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Mcd</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Food</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>20241205201916836536</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>2024-12-10</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>3333</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>RDS PETROZA</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
         <is>
           <t>Food</t>
         </is>

</xml_diff>

<commit_message>
Initial commit for Azure deployment
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
@@ -524,123 +524,48 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>20241205140937284774</t>
+          <t>20241205165544011465</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2022-08-22</t>
+          <t>2018-09-24</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>73.95999999999999</v>
+        <v>23.25</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>RDS PETROZA</t>
+          <t>Berjaya Starbucks Coffee Company SDN BHD</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Transport</t>
+          <t>Food</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>20241205165544011465</t>
+          <t>20241205201244653339</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2018-09-24</t>
+          <t>2024-12-20</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>23.25</v>
+        <v>100</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Berjaya Starbucks Coffee Company SDN BHD</t>
+          <t>Mcd</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
-        <is>
-          <t>Food</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>20241205195645148493</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2024-12-04</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>23.25</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Berjaya Starbucks Coffee Company Sdn Bhd</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Food</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>20241205200912328800</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2024-12-01</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>23.25</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>KFC</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Food</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>20241205201244653339</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2024-12-20</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>100</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Mcd</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
         <is>
           <t>Food</t>
         </is>

</xml_diff>